<commit_message>
created script to setup database for player urls
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CODE\NBA Betting Website\Web Scraping\bet_scrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D86DF4-CAD7-4230-A98D-A31BEEA80B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9A9190-29CF-4F95-896D-C74EE6072A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BFFB2DA5-41FE-4B2D-A995-6CF838EAC496}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{BFFB2DA5-41FE-4B2D-A995-6CF838EAC496}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Player</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>https://www.basketball-reference.com/players/d/davisan02.html</t>
+  </si>
+  <si>
+    <t>Anthony Edwards</t>
   </si>
 </sst>
 </file>
@@ -431,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A456A94-E668-44AE-BBF1-5020185ED805}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -475,6 +478,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>